<commit_message>
Change network line settings
The R + L + (C // G) branch has been changed to (R + L)//C//G branch.
</commit_message>
<xml_diff>
--- a/Examples/HybridPowerSystem/Hybrid_test_v1.xlsx
+++ b/Examples/HybridPowerSystem/Hybrid_test_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\HybridPowerSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E727FF1-C9BD-4659-B86A-17161AFF29BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B47766-CD44-4283-B728-8E0B748B26A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,247 +56,247 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Notes:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The branches can be listed in arbitrary order.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes the parameters for network line impedance.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes the parameters for power flow analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The bus 1 HAVE TO be the slack bus, i.e., type-1 bus.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Samping frequency (Hz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PGi and QGi are in generator convention. PLi and QLi are in load convention.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self branch HAS TO be GC.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mutual branch HAS TO be RL.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes the parameters for network line impedance in IEEE form.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes basic settings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PGi (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QGi (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PLi (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QLi (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qmin (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qmax (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vsp (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summaries advanced settings.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For using this sheet, please set enable from 0 to 1, then this sheet will over-write "NetworkLine"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable (create simulink model)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable (plot pole map)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable (plot admittance)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable (print output)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discretization damping flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discretization method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linearization times</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Direct feedthrough</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power flow algorithm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Base frequency (Hz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Base power (VA)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Base voltage (V)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turns ratio (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>From bus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To bus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>theta (rad)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The transformer is added between FromBus and branch.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FromBus should NOT equal to ToBus in this list.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The transformer is added by turn ratio, which is connected between FromBus and Zbranch in the layout.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For active device (SG, VSI, etc), please use PGi and QGi. For load, please use PLi and QLi.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable (participation)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The branches can be listed in arbitrary order.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User data:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In this form, a pi-circuit between two buses, i.e., series R+jX impedance with parallel G/2+jB/2 admittance at two terminals.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In this form, Zbranch = R+jwL+1/(G+jwC)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC bus type: 1-slack bus, 2-PV bus, 3-PQ bus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC bus type: 1-slack bus (V bus), 2-NaN, 3-P bus (I bus)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bus No.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bus type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turns ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area type: 1-AC, 2-DC.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC or DC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area No.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3, 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes the apparatuses connected to buses.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>inf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Notes:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The branches can be listed in arbitrary order.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summarizes the parameters for network line impedance.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summarizes the parameters for power flow analysis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The bus 1 HAVE TO be the slack bus, i.e., type-1 bus.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Samping frequency (Hz)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PGi and QGi are in generator convention. PLi and QLi are in load convention.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self branch HAS TO be GC.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mutual branch HAS TO be RL.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summarizes the parameters for network line impedance in IEEE form.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summarizes basic settings</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PGi (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>QGi (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PLi (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>QLi (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qmin (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qmax (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vsp (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summaries advanced settings.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>For using this sheet, please set enable from 0 to 1, then this sheet will over-write "NetworkLine"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable (create simulink model)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable (plot pole map)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable (plot admittance)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable (print output)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discretization damping flag</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discretization method</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Linearization times</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Direct feedthrough</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Power flow algorithm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Base frequency (Hz)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Base power (VA)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Base voltage (V)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Turns ratio (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>From bus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>To bus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>theta (rad)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The transformer is added between FromBus and branch.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FromBus should NOT equal to ToBus in this list.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The transformer is added by turn ratio, which is connected between FromBus and Zbranch in the layout.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>For active device (SG, VSI, etc), please use PGi and QGi. For load, please use PLi and QLi.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable (participation)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The branches can be listed in arbitrary order.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User data:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>In this form, a pi-circuit between two buses, i.e., series R+jX impedance with parallel G/2+jB/2 admittance at two terminals.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>In this form, Zbranch = R+jwL+1/(G+jwC)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AC bus type: 1-slack bus, 2-PV bus, 3-PQ bus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DC bus type: 1-slack bus (V bus), 2-NaN, 3-P bus (I bus)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bus No.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bus type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Turns ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Area type: 1-AC, 2-DC.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AC or DC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Area No.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3, 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Parameters</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summarizes the apparatuses connected to buses.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -681,85 +681,85 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="K10" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
@@ -925,7 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -949,23 +949,23 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
@@ -984,7 +984,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>2001</v>
@@ -1026,42 +1026,42 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -1071,15 +1071,15 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>0</v>
@@ -1094,7 +1094,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1108,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0C2B6E-74BD-40FA-8EB6-D64D8C21837A}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1120,50 +1120,50 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -1178,7 +1178,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -1197,8 +1197,8 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" t="s">
-        <v>4</v>
+      <c r="F10">
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1220,8 +1220,8 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" t="s">
-        <v>4</v>
+      <c r="F11">
+        <v>0</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1234,11 +1234,11 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
       </c>
       <c r="E12" s="1">
         <v>1E-4</v>
@@ -1257,11 +1257,11 @@
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>64</v>
       </c>
       <c r="E13" s="1">
         <v>1E-4</v>
@@ -1280,11 +1280,11 @@
       <c r="B14">
         <v>3</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
       </c>
       <c r="E14" s="1">
         <v>1E-4</v>
@@ -1303,11 +1303,11 @@
       <c r="B15">
         <v>4</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
       </c>
       <c r="E15" s="1">
         <v>1E-4</v>
@@ -1344,17 +1344,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <f>B4*1000/2*5</f>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2">
         <v>50</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1407,26 +1407,26 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>0</v>

</xml_diff>

<commit_message>
Change network line settings (#14)
The R + L + (C // G) branch has been changed to (R + L)//C//G branch.
</commit_message>
<xml_diff>
--- a/Examples/HybridPowerSystem/Hybrid_test_v1.xlsx
+++ b/Examples/HybridPowerSystem/Hybrid_test_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\HybridPowerSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E727FF1-C9BD-4659-B86A-17161AFF29BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B47766-CD44-4283-B728-8E0B748B26A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,247 +56,247 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Notes:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The branches can be listed in arbitrary order.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes the parameters for network line impedance.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes the parameters for power flow analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The bus 1 HAVE TO be the slack bus, i.e., type-1 bus.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Samping frequency (Hz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PGi and QGi are in generator convention. PLi and QLi are in load convention.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self branch HAS TO be GC.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mutual branch HAS TO be RL.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes the parameters for network line impedance in IEEE form.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes basic settings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PGi (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QGi (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PLi (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QLi (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qmin (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qmax (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vsp (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summaries advanced settings.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For using this sheet, please set enable from 0 to 1, then this sheet will over-write "NetworkLine"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable (create simulink model)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable (plot pole map)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable (plot admittance)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable (print output)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discretization damping flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discretization method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linearization times</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Direct feedthrough</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power flow algorithm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Base frequency (Hz)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Base power (VA)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Base voltage (V)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turns ratio (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>From bus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To bus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>theta (rad)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The transformer is added between FromBus and branch.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FromBus should NOT equal to ToBus in this list.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The transformer is added by turn ratio, which is connected between FromBus and Zbranch in the layout.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For active device (SG, VSI, etc), please use PGi and QGi. For load, please use PLi and QLi.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable (participation)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The branches can be listed in arbitrary order.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User data:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In this form, a pi-circuit between two buses, i.e., series R+jX impedance with parallel G/2+jB/2 admittance at two terminals.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In this form, Zbranch = R+jwL+1/(G+jwC)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC bus type: 1-slack bus, 2-PV bus, 3-PQ bus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC bus type: 1-slack bus (V bus), 2-NaN, 3-P bus (I bus)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bus No.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bus type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turns ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area type: 1-AC, 2-DC.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC or DC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area No.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3, 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet summarizes the apparatuses connected to buses.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>inf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Notes:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The branches can be listed in arbitrary order.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summarizes the parameters for network line impedance.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summarizes the parameters for power flow analysis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The bus 1 HAVE TO be the slack bus, i.e., type-1 bus.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Samping frequency (Hz)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PGi and QGi are in generator convention. PLi and QLi are in load convention.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self branch HAS TO be GC.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mutual branch HAS TO be RL.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summarizes the parameters for network line impedance in IEEE form.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summarizes basic settings</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PGi (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>QGi (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PLi (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>QLi (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qmin (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qmax (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vsp (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summaries advanced settings.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>For using this sheet, please set enable from 0 to 1, then this sheet will over-write "NetworkLine"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable (create simulink model)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable (plot pole map)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable (plot admittance)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable (print output)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discretization damping flag</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discretization method</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Linearization times</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Direct feedthrough</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Power flow algorithm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Base frequency (Hz)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Base power (VA)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Base voltage (V)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Turns ratio (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>From bus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>To bus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>theta (rad)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The transformer is added between FromBus and branch.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FromBus should NOT equal to ToBus in this list.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The transformer is added by turn ratio, which is connected between FromBus and Zbranch in the layout.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>For active device (SG, VSI, etc), please use PGi and QGi. For load, please use PLi and QLi.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable (participation)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The branches can be listed in arbitrary order.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User data:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>In this form, a pi-circuit between two buses, i.e., series R+jX impedance with parallel G/2+jB/2 admittance at two terminals.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>In this form, Zbranch = R+jwL+1/(G+jwC)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AC bus type: 1-slack bus, 2-PV bus, 3-PQ bus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DC bus type: 1-slack bus (V bus), 2-NaN, 3-P bus (I bus)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bus No.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bus type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Turns ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Area type: 1-AC, 2-DC.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AC or DC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Area No.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3, 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Parameters</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This sheet summarizes the apparatuses connected to buses.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -681,85 +681,85 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="K10" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
@@ -925,7 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -949,23 +949,23 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
@@ -984,7 +984,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>2001</v>
@@ -1026,42 +1026,42 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -1071,15 +1071,15 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>0</v>
@@ -1094,7 +1094,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1108,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0C2B6E-74BD-40FA-8EB6-D64D8C21837A}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1120,50 +1120,50 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -1178,7 +1178,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -1197,8 +1197,8 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" t="s">
-        <v>4</v>
+      <c r="F10">
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1220,8 +1220,8 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" t="s">
-        <v>4</v>
+      <c r="F11">
+        <v>0</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1234,11 +1234,11 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
       </c>
       <c r="E12" s="1">
         <v>1E-4</v>
@@ -1257,11 +1257,11 @@
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>64</v>
       </c>
       <c r="E13" s="1">
         <v>1E-4</v>
@@ -1280,11 +1280,11 @@
       <c r="B14">
         <v>3</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
       </c>
       <c r="E14" s="1">
         <v>1E-4</v>
@@ -1303,11 +1303,11 @@
       <c r="B15">
         <v>4</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
       </c>
       <c r="E15" s="1">
         <v>1E-4</v>
@@ -1344,17 +1344,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <f>B4*1000/2*5</f>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2">
         <v>50</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1407,26 +1407,26 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>0</v>

</xml_diff>